<commit_message>
Fix blue tab color in EGGRA
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/EGGRA/Exogenous GDP Growth Rate Adjustment.xlsx
+++ b/InputData/ctrl-settings/EGGRA/Exogenous GDP Growth Rate Adjustment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\ctrl-settings\EGGRA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24F8205-3026-4E9D-B27B-59DF76E583C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D77B80-46D1-401E-A779-175C6F49CDE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19845" yWindow="1005" windowWidth="15990" windowHeight="20745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9555" yWindow="345" windowWidth="22590" windowHeight="21675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -877,6 +877,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B09BF19-5F77-48B9-A755-C990DA6AE4FD}">
+  <sheetPr>
+    <tabColor theme="8" tint="-0.249977111117893"/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>